<commit_message>
changes to binary files
</commit_message>
<xml_diff>
--- a/test-data/bewertung.xlsx
+++ b/test-data/bewertung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swehr/devel/check-assignments/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCFA1FD-B189-2946-B583-81A46E3D20A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDA867C-732B-104B-A297-0109ED416333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="4000" windowWidth="42680" windowHeight="24180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6680" yWindow="28800" windowWidth="27120" windowHeight="22400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ergebnis" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>bar</t>
+  </si>
+  <si>
+    <t>blub</t>
+  </si>
+  <si>
+    <t>hello</t>
   </si>
 </sst>
 </file>
@@ -2146,17 +2152,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2B15E0-2AB4-9643-8338-2F6129F3E480}">
-  <dimension ref="A1:AW4"/>
+  <dimension ref="A1:AW7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.1640625" bestFit="1" customWidth="1"/>
@@ -2422,6 +2428,26 @@
         <v>50</v>
       </c>
     </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="A5" s="16"/>
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="A6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="A7" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7">
+        <f>1+2</f>
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>